<commit_message>
Add customer and product analysis
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub_Repository\online-pet-supply-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F91E9512-11B8-4555-9D45-D39B2F7C8D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2BB2E3-62CC-4871-AEB3-3CE770872D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,13 +524,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>